<commit_message>
Update Streamlit app with latest changes
</commit_message>
<xml_diff>
--- a/data/EDM_DATA.xlsx
+++ b/data/EDM_DATA.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1787,6 +1787,198 @@
         <v>0.009974036213122539</v>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:39</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>-0.1226930397070828</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-0.001828903161391997</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.008975747528043098</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:40</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>-0.1227613595774164</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-0.002091892289527995</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.01027214166207885</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:41</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>-0.1216129350903793</v>
+      </c>
+      <c r="C88" t="n">
+        <v>-0.002015566730399995</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.009804759438178507</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:42</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>-0.1218764545902377</v>
+      </c>
+      <c r="C89" t="n">
+        <v>-0.001896371311469995</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.009244920481144097</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:43</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>-0.1226051998737967</v>
+      </c>
+      <c r="C90" t="n">
+        <v>-0.001937419075695996</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.009501506120600561</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:44</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>-0.1231062122562434</v>
+      </c>
+      <c r="C91" t="n">
+        <v>-0.001992385625571996</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.00981100190871818</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:45</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>-0.1219480277877301</v>
+      </c>
+      <c r="C92" t="n">
+        <v>-0.001787450487037997</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.008719042466500054</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:46</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>-0.1228491994107026</v>
+      </c>
+      <c r="C93" t="n">
+        <v>-0.001789576265209996</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.008793920458617726</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:47</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>-0.1248857822120772</v>
+      </c>
+      <c r="C94" t="n">
+        <v>-0.001851679356091995</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.009249936991660167</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:48</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>-0.1261480731496704</v>
+      </c>
+      <c r="C95" t="n">
+        <v>-0.001939342398803996</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.009785772271463346</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:49</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>-0.1254323411747464</v>
+      </c>
+      <c r="C96" t="n">
+        <v>-0.002070583894041995</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.01038872741713642</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2024-12-18 23:46:50</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>-0.1250386885885382</v>
+      </c>
+      <c r="C97" t="n">
+        <v>-0.001975176945131996</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.009878941397984793</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>